<commit_message>
Updated - fixed pricing error on o-rings
</commit_message>
<xml_diff>
--- a/extruder/extruder_BOM.xlsx
+++ b/extruder/extruder_BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="4440" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2504,11 +2504,11 @@
         <v>150</v>
       </c>
       <c r="G81">
-        <v>15</v>
+        <v>0.65</v>
       </c>
       <c r="H81">
         <f>A81*G81</f>
-        <v>45</v>
+        <v>1.9500000000000002</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="19" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="H86">
         <f>SUM(H5:H84)</f>
-        <v>399.32000000000005</v>
+        <v>356.27000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2592,8 +2592,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" fitToWidth="2" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <rowBreaks count="2" manualBreakCount="2">
-    <brk id="2" max="16383" man="1"/>
+  <rowBreaks count="1" manualBreakCount="1">
     <brk id="131" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="2" manualBreakCount="2">

</xml_diff>

<commit_message>
Added polycarbonate tubing to BOM
</commit_message>
<xml_diff>
--- a/extruder/extruder_BOM.xlsx
+++ b/extruder/extruder_BOM.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="171">
   <si>
     <t>Size</t>
   </si>
@@ -278,9 +278,6 @@
     <t>38mm</t>
   </si>
   <si>
-    <t>IV.) Motors with Gearboxes</t>
-  </si>
-  <si>
     <t>Motor</t>
   </si>
   <si>
@@ -338,9 +335,6 @@
     <t>wormGear_nut_coupling.stl</t>
   </si>
   <si>
-    <t>V.) O-Rings</t>
-  </si>
-  <si>
     <t>bearing_cover.stl</t>
   </si>
   <si>
@@ -365,9 +359,6 @@
     <t>gasket_B.dxf</t>
   </si>
   <si>
-    <t>VI.) Nozzles</t>
-  </si>
-  <si>
     <t>tubeHolder_grip.dxf</t>
   </si>
   <si>
@@ -522,13 +513,40 @@
   </si>
   <si>
     <t>Tube Base</t>
+  </si>
+  <si>
+    <t>VII.) Nozzles</t>
+  </si>
+  <si>
+    <t>VI.) O-Rings</t>
+  </si>
+  <si>
+    <t>V.) Motors with Gearboxes</t>
+  </si>
+  <si>
+    <t>IV.) Polycarbonate Tubing</t>
+  </si>
+  <si>
+    <t>2.75in</t>
+  </si>
+  <si>
+    <t>3in</t>
+  </si>
+  <si>
+    <t>500mm</t>
+  </si>
+  <si>
+    <t>Polycarbonate</t>
+  </si>
+  <si>
+    <t>https://www.eplastics.com/Clear-Polycarbonate-Rigid-Tubing-2-3-4-ID-x-3-OD-x-1-8-Wall-x-8ft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -616,6 +634,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="19"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -638,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -656,6 +679,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -934,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,7 +983,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -999,10 +1028,10 @@
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1016,13 +1045,13 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G6">
         <v>0.1</v>
@@ -1043,13 +1072,13 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G7">
         <v>0.05</v>
@@ -1070,13 +1099,13 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G8">
         <v>0.06</v>
@@ -1103,7 +1132,7 @@
         <v>47</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G9">
         <v>0.06</v>
@@ -1130,7 +1159,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G10">
         <v>7.0000000000000007E-2</v>
@@ -1157,7 +1186,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G11">
         <v>0.1</v>
@@ -1207,13 +1236,13 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G14">
         <v>0.1</v>
@@ -1240,7 +1269,7 @@
         <v>24</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G15">
         <v>0.08</v>
@@ -1267,7 +1296,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G16">
         <v>0.09</v>
@@ -1294,7 +1323,7 @@
         <v>22</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G17">
         <v>0.12</v>
@@ -1321,7 +1350,7 @@
         <v>23</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G18">
         <v>0.11</v>
@@ -1348,7 +1377,7 @@
         <v>22</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G19">
         <v>0.18</v>
@@ -1404,7 +1433,7 @@
         <v>28</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G22">
         <v>0.14000000000000001</v>
@@ -1431,7 +1460,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G23">
         <v>0.22</v>
@@ -1487,7 +1516,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G26">
         <v>0.11</v>
@@ -1514,7 +1543,7 @@
         <v>20</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G27">
         <v>0.05</v>
@@ -1541,7 +1570,7 @@
         <v>35</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G28">
         <v>0.22</v>
@@ -1553,7 +1582,7 @@
     </row>
     <row r="30" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1575,7 +1604,7 @@
         <v>18</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1583,11 +1612,11 @@
         <v>1</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
@@ -1609,13 +1638,13 @@
       </c>
       <c r="C33" s="6"/>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G33">
         <v>40</v>
@@ -1630,11 +1659,11 @@
         <v>1</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -1652,11 +1681,11 @@
         <v>1</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -1674,11 +1703,11 @@
         <v>1</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
         <v>61</v>
@@ -1696,11 +1725,11 @@
         <v>1</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E37" t="s">
         <v>61</v>
@@ -1718,11 +1747,11 @@
         <v>1</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E38" t="s">
         <v>61</v>
@@ -1740,11 +1769,11 @@
         <v>1</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E39" t="s">
         <v>62</v>
@@ -1762,11 +1791,11 @@
         <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E40" t="s">
         <v>62</v>
@@ -1784,11 +1813,11 @@
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E41" t="s">
         <v>62</v>
@@ -1806,11 +1835,11 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E42" t="s">
         <v>62</v>
@@ -1828,17 +1857,17 @@
         <v>1</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
         <v>62</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G43">
         <v>46</v>
@@ -1853,11 +1882,11 @@
         <v>1</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E44" t="s">
         <v>24</v>
@@ -1875,17 +1904,17 @@
         <v>1</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E45" t="s">
         <v>19</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G45">
         <v>1.54</v>
@@ -1900,11 +1929,11 @@
         <v>1</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E46" t="s">
         <v>19</v>
@@ -1916,11 +1945,11 @@
         <v>2</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
@@ -1981,7 +2010,7 @@
         <v>42</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G52">
         <v>6.69</v>
@@ -2008,7 +2037,7 @@
         <v>49</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G53">
         <v>18.14</v>
@@ -2052,19 +2081,19 @@
         <v>1</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G56">
         <v>0.12</v>
@@ -2091,7 +2120,7 @@
         <v>42</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G57">
         <v>0.3</v>
@@ -2121,7 +2150,7 @@
         <v>29</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>18</v>
@@ -2141,13 +2170,13 @@
         <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E60" t="s">
         <v>62</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G60">
         <v>40</v>
@@ -2175,7 +2204,7 @@
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>18</v>
@@ -2192,13 +2221,13 @@
         <v>65</v>
       </c>
       <c r="D63" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E63" t="s">
         <v>68</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G63">
         <v>4.99</v>
@@ -2254,7 +2283,7 @@
         <v>61</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G66">
         <v>20.48</v>
@@ -2310,7 +2339,7 @@
         <v>49</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G69">
         <v>2.4</v>
@@ -2362,7 +2391,7 @@
         <v>20</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G72">
         <v>2</v>
@@ -2372,30 +2401,35 @@
         <v>4</v>
       </c>
     </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="F73" s="9"/>
+    </row>
     <row r="74" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="7"/>
-      <c r="E74" s="7"/>
+      <c r="A74" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>86</v>
+      <c r="B75" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>6</v>
@@ -2405,115 +2439,115 @@
       <c r="A76">
         <v>1</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G76">
+        <v>25</v>
+      </c>
+      <c r="H76">
+        <f>G76*A76</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D80" t="s">
+        <v>88</v>
+      </c>
+      <c r="E80" t="s">
+        <v>103</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G80">
+        <v>30</v>
+      </c>
+      <c r="H80">
+        <f t="shared" ref="H80:H81" si="7">A80*G80</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="C81" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D81" t="s">
         <v>89</v>
       </c>
-      <c r="E76" t="s">
-        <v>105</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G76">
-        <v>30</v>
-      </c>
-      <c r="H76">
-        <f t="shared" ref="H76:H77" si="7">A76*G76</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>1</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D77" t="s">
-        <v>90</v>
-      </c>
-      <c r="E77" t="s">
-        <v>106</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G77">
+      <c r="E81" t="s">
+        <v>104</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G81">
         <v>100</v>
       </c>
-      <c r="H77">
+      <c r="H81">
         <f t="shared" si="7"/>
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>3</v>
-      </c>
-      <c r="B81" t="s">
-        <v>56</v>
-      </c>
-      <c r="C81" t="s">
-        <v>107</v>
-      </c>
-      <c r="D81" t="s">
-        <v>108</v>
-      </c>
-      <c r="E81" t="s">
-        <v>109</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="G81">
-        <v>0.65</v>
-      </c>
-      <c r="H81">
-        <f>A81*G81</f>
-        <v>1.9500000000000002</v>
-      </c>
-    </row>
     <row r="83" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -2521,34 +2555,94 @@
       <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B84" s="10"/>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
-      <c r="G84">
+      <c r="A84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H84">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85" t="s">
+        <v>56</v>
+      </c>
+      <c r="C85" t="s">
+        <v>105</v>
+      </c>
+      <c r="D85" t="s">
+        <v>106</v>
+      </c>
+      <c r="E85" t="s">
+        <v>107</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G85">
+        <v>0.65</v>
+      </c>
+      <c r="H85">
+        <f>A85*G85</f>
+        <v>1.9500000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="G88">
         <v>6</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G86" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H86">
-        <f>SUM(H5:H84)</f>
-        <v>356.27000000000004</v>
-      </c>
+      <c r="H88">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G90" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H90">
+        <f>SUM(H5:H88)</f>
+        <v>381.27000000000004</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="24" x14ac:dyDescent="0.25">
+      <c r="F93" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A74:D74"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -2579,21 +2673,22 @@
     <hyperlink ref="F66" r:id="rId25"/>
     <hyperlink ref="F69" r:id="rId26"/>
     <hyperlink ref="F72" r:id="rId27"/>
-    <hyperlink ref="F77" r:id="rId28"/>
-    <hyperlink ref="F76" r:id="rId29"/>
-    <hyperlink ref="F81" r:id="rId30"/>
-    <hyperlink ref="A84" r:id="rId31"/>
-    <hyperlink ref="B84" r:id="rId32" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
-    <hyperlink ref="C84" r:id="rId33" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
-    <hyperlink ref="D84" r:id="rId34" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
-    <hyperlink ref="E84" r:id="rId35" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
+    <hyperlink ref="F81" r:id="rId28"/>
+    <hyperlink ref="F80" r:id="rId29"/>
+    <hyperlink ref="F85" r:id="rId30"/>
+    <hyperlink ref="A88" r:id="rId31"/>
+    <hyperlink ref="B88" r:id="rId32" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
+    <hyperlink ref="C88" r:id="rId33" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
+    <hyperlink ref="D88" r:id="rId34" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
+    <hyperlink ref="E88" r:id="rId35" display="https://www.aliexpress.com/item/32738744288.html?spm=a2g0o.productlist.0.0.1e304f6eNn0Dlt&amp;algo_pvid=df21f6af-004c-4882-b7eb-044cfd1a0941&amp;algo_expid=df21f6af-004c-4882-b7eb-044cfd1a0941-18&amp;btsid=0ab6f81e15856117217356590e31f4&amp;ws_ab_test=searchweb0_"/>
     <hyperlink ref="F45" r:id="rId36"/>
     <hyperlink ref="F14" r:id="rId37"/>
+    <hyperlink ref="F76" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" fitToWidth="2" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="131" max="16383" man="1"/>
+    <brk id="135" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="2" manualBreakCount="2">
     <brk id="11" max="1048575" man="1"/>

</xml_diff>